<commit_message>
Update Eksport -sortering varegrupper (Justerte SITC grupper).xlsx
</commit_message>
<xml_diff>
--- a/Eksport -sortering varegrupper (Justerte SITC grupper).xlsx
+++ b/Eksport -sortering varegrupper (Justerte SITC grupper).xlsx
@@ -562,8 +562,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005BAF6522D6B39A4F809F4AA1655E5CD6" ma:contentTypeVersion="11" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="ca392f09ec4657bc601066d7bc537d21">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="712f17e0-2077-4e3f-8ea2-c75d02de46ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="345553e69f630f0ba71e029dc9be3dcc" ns1:_="" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005BAF6522D6B39A4F809F4AA1655E5CD6" ma:contentTypeVersion="12" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="e4a524b860cf13a8c93835716f8e4da0">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="712f17e0-2077-4e3f-8ea2-c75d02de46ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="810e635cb89f261f8aa95246a976651c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="712f17e0-2077-4e3f-8ea2-c75d02de46ee"/>
     <xsd:element name="properties">
@@ -584,6 +584,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -660,6 +661,11 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -781,5 +787,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80088AF0-2517-41B3-B02F-7B09AA4C9450}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1FEDA7D-BE1C-4137-AA7B-62DFEF6A1AD7}"/>
 </file>
</xml_diff>